<commit_message>
Conceptual Data Model updated
</commit_message>
<xml_diff>
--- a/02_IR_DED/eForms_20180221_BTs_descriptions.xlsx
+++ b/02_IR_DED/eForms_20180221_BTs_descriptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showObjects="none" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ePO\ePO-everis\02_IR_DED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ePO\epo-everis\02_IR_DED\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6858,9 +6858,9 @@
   </sheetPr>
   <dimension ref="A1:AF437"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE126" sqref="AE126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50000,8 +50000,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c2ecfd70-f0a7-4227-9d3f-c0584232298e" ContentTypeId="0x010100AAE994419BC24CED8BF9A98B0A371F99" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Document_x0020_Description xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <UnitDir xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AresNumber xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </AresNumber>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50182,16 +50190,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Document_x0020_Description xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <UnitDir xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AresNumber xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </AresNumber>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c2ecfd70-f0a7-4227-9d3f-c0584232298e" ContentTypeId="0x010100AAE994419BC24CED8BF9A98B0A371F99" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50204,9 +50204,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC774358-9406-4AC1-A9B3-845F659D4FB0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2180D379-9015-4716-A545-2BFA70970FEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -50230,17 +50238,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2180D379-9015-4716-A545-2BFA70970FEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC774358-9406-4AC1-A9B3-845F659D4FB0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>